<commit_message>
Implemented Custom JWT Roles bases Authentication & Authorization
</commit_message>
<xml_diff>
--- a/Authorization-Policy-Group-Roles-Permissions.xlsx
+++ b/Authorization-Policy-Group-Roles-Permissions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="167">
   <si>
     <t>Admin</t>
   </si>
@@ -442,9 +442,6 @@
     <t>CQRS with MediatR</t>
   </si>
   <si>
-    <t>Fluent Validations</t>
-  </si>
-  <si>
     <t>Swagger/ Open API</t>
   </si>
   <si>
@@ -497,6 +494,36 @@
   </si>
   <si>
     <t>https://code-maze.com/swagger-ui-asp-net-core-web-api/#Extending</t>
+  </si>
+  <si>
+    <t>https://www.toptal.com/asp-dot-net/asp-net-web-api-tutorial</t>
+  </si>
+  <si>
+    <t>Repository Pattern</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Non Functional</t>
+  </si>
+  <si>
+    <t>Others/Misc</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>Fluent Validations / Data Annotations</t>
+  </si>
+  <si>
+    <t>https://code-maze.com/async-generic-repository-pattern/</t>
+  </si>
+  <si>
+    <t>Async Repository Pattern</t>
+  </si>
+  <si>
+    <t>https://www.thereformedprogrammer.net/a-better-way-to-handle-authorization-in-asp-net-core/</t>
   </si>
 </sst>
 </file>
@@ -690,7 +717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -769,6 +796,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -802,6 +835,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1086,12 +1120,12 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="17"/>
     <col min="4" max="16384" width="9.140625" style="16"/>
@@ -1105,11 +1139,11 @@
         <v>130</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>125</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1118,7 +1152,7 @@
       <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="14" t="s">
         <v>124</v>
       </c>
@@ -1138,99 +1172,128 @@
         <v>127</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>159</v>
+      </c>
       <c r="B8" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
       <c r="B9" s="21" t="s">
         <v>133</v>
       </c>
       <c r="C9" s="22"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="30"/>
       <c r="B10" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="22"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="22"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
-        <v>134</v>
-      </c>
       <c r="C11" s="22"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
       <c r="B12" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
+      <c r="B13" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="22"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="22"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="22"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C14" s="22"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+      <c r="B17" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="22"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+      <c r="B18" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="22"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="22"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C17" s="22"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="C18" s="22"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="21" t="s">
+      <c r="C19" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="29"/>
+      <c r="B20" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="22"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
-        <v>144</v>
-      </c>
       <c r="C20" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A8:A13"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="iconSet" priority="1">
@@ -1250,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H18" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1269,41 +1332,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="35" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="37" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="33"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1316,13 +1379,13 @@
       <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="36"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="32" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1348,7 +1411,7 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1372,7 +1435,7 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="32" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1398,7 +1461,7 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1420,7 +1483,7 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="32" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1444,7 +1507,7 @@
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="32"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1466,7 +1529,7 @@
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="31"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1739,11 +1802,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1754,20 +1817,21 @@
     <col min="4" max="6" width="9.140625" style="18"/>
     <col min="7" max="7" width="15.85546875" style="18" customWidth="1"/>
     <col min="8" max="8" width="51.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="18"/>
+    <col min="9" max="9" width="57" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1997,7 +2061,7 @@
       <c r="G16" s="13"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>83</v>
@@ -2015,7 +2079,7 @@
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>82</v>
@@ -2029,7 +2093,7 @@
       <c r="G18" s="13"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>1</v>
@@ -2043,7 +2107,7 @@
       <c r="G19" s="13"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>2</v>
@@ -2057,7 +2121,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
         <v>18</v>
@@ -2071,7 +2135,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>3</v>
@@ -2085,7 +2149,7 @@
       <c r="G22" s="13"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>63</v>
@@ -2099,7 +2163,7 @@
       <c r="G23" s="13"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>64</v>
@@ -2113,7 +2177,7 @@
       <c r="G24" s="13"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="8" t="s">
         <v>65</v>
@@ -2127,7 +2191,7 @@
       <c r="G25" s="13"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="8" t="s">
         <v>66</v>
@@ -2141,7 +2205,7 @@
       <c r="G26" s="13"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="8"/>
       <c r="C27" s="13"/>
@@ -2151,7 +2215,7 @@
       <c r="G27" s="13"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="12" t="s">
         <v>14</v>
@@ -2163,7 +2227,7 @@
       <c r="G28" s="11"/>
       <c r="H28" s="12"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>37</v>
@@ -2176,8 +2240,12 @@
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="18" t="str">
+        <f>CONCATENATE("public ", IF(C29="INT","int",IF(C29="VARCHAR","string",IF(C29="DATE","DateTime",IF(C29="DATETIME","DateTime",IF(C29="BIT","bool","")))))," ",B29," { get; set; }")</f>
+        <v>public int Id { get; set; }</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>39</v>
@@ -2192,8 +2260,12 @@
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="18" t="str">
+        <f t="shared" ref="I30:I49" si="0">CONCATENATE("public ", IF(C30="INT","int",IF(C30="VARCHAR","string",IF(C30="DATE","DateTime",IF(C30="DATETIME","DateTime",IF(C30="BIT","bool","")))))," ",B30," { get; set; }")</f>
+        <v>public string UserName { get; set; }</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
         <v>112</v>
@@ -2208,8 +2280,12 @@
       <c r="H31" s="8" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public  PasswordHash { get; set; }</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="s">
         <v>40</v>
@@ -2222,8 +2298,12 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="8"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public  PasswordSalt { get; set; }</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="s">
         <v>113</v>
@@ -2236,8 +2316,12 @@
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool RememberPassword { get; set; }</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>114</v>
@@ -2250,8 +2334,12 @@
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="8"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public int WrongPasswordAttempt { get; set; }</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
         <v>115</v>
@@ -2264,8 +2352,12 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public DateTime WrongPasswordAttemptDate { get; set; }</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="s">
         <v>117</v>
@@ -2278,8 +2370,12 @@
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ForceChangePassword { get; set; }</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="8" t="s">
         <v>116</v>
@@ -2292,8 +2388,12 @@
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool IsActive { get; set; }</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="8" t="s">
         <v>41</v>
@@ -2308,8 +2408,12 @@
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public string FirstName { get; set; }</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="8" t="s">
         <v>42</v>
@@ -2324,8 +2428,12 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="8"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public string LastName { get; set; }</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="8" t="s">
         <v>43</v>
@@ -2342,8 +2450,12 @@
         <v>119</v>
       </c>
       <c r="H40" s="8"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public int Gender { get; set; }</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="8" t="s">
         <v>44</v>
@@ -2356,8 +2468,12 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public DateTime DateOfBirth { get; set; }</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="B42" s="8" t="s">
         <v>45</v>
@@ -2370,8 +2486,12 @@
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="8"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public DateTime DateOfJoining { get; set; }</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="8" t="s">
         <v>46</v>
@@ -2384,8 +2504,12 @@
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="8"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public string Designation { get; set; }</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="8" t="s">
         <v>63</v>
@@ -2398,8 +2522,12 @@
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public int CreatedBy { get; set; }</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="8" t="s">
         <v>64</v>
@@ -2412,8 +2540,12 @@
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="8"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public DateTime CreatedDate { get; set; }</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="8" t="s">
         <v>65</v>
@@ -2426,8 +2558,12 @@
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="8"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public int ModifiedBy { get; set; }</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="B47" s="8" t="s">
         <v>66</v>
@@ -2440,8 +2576,12 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="8"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public DateTime ModifiedDate { get; set; }</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="8" t="s">
         <v>80</v>
@@ -2454,8 +2594,12 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="8"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public int DeletedBy { get; set; }</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="8" t="s">
         <v>81</v>
@@ -2468,8 +2612,12 @@
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="8"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>public DateTime DeletedDate { get; set; }</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="8"/>
       <c r="C50" s="13"/>
@@ -2479,7 +2627,7 @@
       <c r="G50" s="13"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="11"/>
       <c r="B51" s="12" t="s">
         <v>107</v>
@@ -2491,7 +2639,7 @@
       <c r="G51" s="11"/>
       <c r="H51" s="12"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
       <c r="B52" s="8" t="s">
         <v>37</v>
@@ -2505,7 +2653,7 @@
       <c r="G52" s="13"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="B53" s="8" t="s">
         <v>108</v>
@@ -2523,7 +2671,7 @@
       </c>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
       <c r="B54" s="8" t="s">
         <v>109</v>
@@ -2541,7 +2689,7 @@
       </c>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
       <c r="B55" s="8" t="s">
         <v>63</v>
@@ -2555,7 +2703,7 @@
       <c r="G55" s="13"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
       <c r="B56" s="8" t="s">
         <v>64</v>
@@ -2569,7 +2717,7 @@
       <c r="G56" s="13"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="13"/>
       <c r="B57" s="8" t="s">
         <v>65</v>
@@ -2583,7 +2731,7 @@
       <c r="G57" s="13"/>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="B58" s="8" t="s">
         <v>66</v>
@@ -2597,7 +2745,7 @@
       <c r="G58" s="13"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
       <c r="B59" s="8" t="s">
         <v>80</v>
@@ -2611,7 +2759,7 @@
       <c r="G59" s="13"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="13"/>
       <c r="B60" s="8" t="s">
         <v>81</v>
@@ -2625,7 +2773,7 @@
       <c r="G60" s="13"/>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="13"/>
       <c r="B61" s="8"/>
       <c r="C61" s="13"/>
@@ -2635,7 +2783,7 @@
       <c r="G61" s="13"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="11"/>
       <c r="B62" s="12" t="s">
         <v>91</v>
@@ -2647,7 +2795,7 @@
       <c r="G62" s="11"/>
       <c r="H62" s="12"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
       <c r="B63" s="8" t="s">
         <v>37</v>
@@ -2659,7 +2807,7 @@
       <c r="G63" s="13"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="13"/>
       <c r="B64" s="8" t="s">
         <v>92</v>
@@ -2993,10 +3141,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3009,7 +3157,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3017,10 +3165,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>149</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3028,10 +3176,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>151</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3039,10 +3187,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>153</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3050,10 +3198,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3061,7 +3209,34 @@
         <v>5</v>
       </c>
       <c r="C6" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3071,6 +3246,9 @@
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5" location="Extending"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented JWT Policy Based Authentication with Permission
</commit_message>
<xml_diff>
--- a/Authorization-Policy-Group-Roles-Permissions.xlsx
+++ b/Authorization-Policy-Group-Roles-Permissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="168">
   <si>
     <t>Admin</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>https://www.thereformedprogrammer.net/a-better-way-to-handle-authorization-in-asp-net-core/</t>
+  </si>
+  <si>
+    <t>https://www.c-sharpcorner.com/article/policy-based-authorization-with-angular-and-asp-net-core-using-jwt/</t>
   </si>
 </sst>
 </file>
@@ -799,6 +802,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -835,7 +839,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1119,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1143,7 +1146,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>125</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1152,7 +1155,7 @@
       <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="14" t="s">
         <v>124</v>
       </c>
@@ -1188,7 +1191,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="31" t="s">
         <v>159</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -1199,42 +1202,46 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="21" t="s">
         <v>140</v>
       </c>
       <c r="C11" s="22"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="21" t="s">
         <v>141</v>
       </c>
       <c r="C12" s="22"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="21" t="s">
         <v>142</v>
       </c>
       <c r="C13" s="22"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
         <v>160</v>
       </c>
       <c r="B14" s="21" t="s">
@@ -1243,35 +1250,39 @@
       <c r="C14" s="22"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="21" t="s">
         <v>137</v>
       </c>
       <c r="C16" s="22"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="21" t="s">
         <v>138</v>
       </c>
       <c r="C17" s="22"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="30" t="s">
         <v>161</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -1282,7 +1293,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="29"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="21" t="s">
         <v>143</v>
       </c>
@@ -1314,7 +1325,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1332,41 +1343,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="37" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="38" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="35"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1379,13 +1390,13 @@
       <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="38"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1411,7 +1422,7 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1435,7 +1446,7 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1461,7 +1472,7 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="33"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1483,7 +1494,7 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="33" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1507,7 +1518,7 @@
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="34"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1529,7 +1540,7 @@
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="33"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1822,16 +1833,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -3141,10 +3152,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3235,8 +3246,13 @@
       <c r="B9" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="29" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="25" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3249,6 +3265,7 @@
     <hyperlink ref="C7" r:id="rId6"/>
     <hyperlink ref="C8" r:id="rId7"/>
     <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Config Key Values Classes and Seed data
</commit_message>
<xml_diff>
--- a/Authorization-Policy-Group-Roles-Permissions.xlsx
+++ b/Authorization-Policy-Group-Roles-Permissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="172">
   <si>
     <t>Admin</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>OrderId</t>
   </si>
   <si>
     <t>VARCHAR</t>
@@ -527,6 +524,21 @@
   </si>
   <si>
     <t>https://www.c-sharpcorner.com/article/policy-based-authorization-with-angular-and-asp-net-core-using-jwt/</t>
+  </si>
+  <si>
+    <t>https://developer.okta.com/blog/2018/05/11/policy-based-authorization-in-aspnet-core</t>
+  </si>
+  <si>
+    <t>Data Seeding</t>
+  </si>
+  <si>
+    <t>Filter Attributes</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>User to Orderby</t>
   </si>
 </sst>
 </file>
@@ -720,7 +732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -804,6 +816,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -837,6 +852,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1120,11 +1138,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1136,157 +1152,155 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
-        <v>125</v>
+      <c r="A2" s="32" t="s">
+        <v>124</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="14" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="14" t="s">
-        <v>124</v>
       </c>
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="22"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" s="22"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="32"/>
+      <c r="B11" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="32"/>
+      <c r="B12" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="22"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="32"/>
+      <c r="B17" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="32"/>
+      <c r="B18" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="22"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="21" t="s">
         <v>162</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="22"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="22"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="22"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="C14" s="22"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="22"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="C17" s="22"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="C18" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>139</v>
       </c>
       <c r="C19" s="22">
         <v>1</v>
@@ -1295,16 +1309,44 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20" s="21" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="C20" s="22"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="30"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="30"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="31"/>
+      <c r="B24" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A8:A14"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="iconSet" priority="1">
@@ -1325,7 +1367,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1343,41 +1385,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="38" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="39" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="36"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1390,13 +1432,13 @@
       <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="39"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1422,7 +1464,7 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1446,7 +1488,7 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="34" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1472,7 +1514,7 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1494,7 +1536,7 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1518,7 +1560,7 @@
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1540,7 +1582,7 @@
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1563,10 +1605,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -1581,7 +1623,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1595,7 +1637,7 @@
         <v>20</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>6</v>
@@ -1612,10 +1654,10 @@
         <v>13</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1629,10 +1671,10 @@
         <v>12</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1646,10 +1688,10 @@
         <v>11</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1663,10 +1705,10 @@
         <v>10</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1680,10 +1722,10 @@
         <v>15</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1697,10 +1739,10 @@
         <v>16</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1714,10 +1756,10 @@
         <v>16</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1731,10 +1773,10 @@
         <v>17</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1743,34 +1785,34 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H23" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H24" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H26" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1779,10 +1821,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H28" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1815,9 +1857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1833,16 +1875,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1904,7 +1946,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="13">
         <v>20</v>
@@ -1913,16 +1955,16 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="13">
         <v>500</v>
@@ -1984,7 +2026,7 @@
         <v>34</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -1994,7 +2036,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="13">
         <v>120</v>
@@ -2007,10 +2049,10 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="13">
         <v>500</v>
@@ -2023,7 +2065,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="8" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>38</v>
@@ -2032,7 +2074,9 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
@@ -2055,7 +2099,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2075,7 +2119,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>38</v>
@@ -2086,17 +2130,17 @@
         <v>34</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -2110,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
@@ -2124,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
@@ -2138,7 +2182,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -2152,7 +2196,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
@@ -2163,7 +2207,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>38</v>
@@ -2177,10 +2221,10 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -2191,7 +2235,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>38</v>
@@ -2205,10 +2249,10 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
@@ -2262,7 +2306,7 @@
         <v>39</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="13">
         <v>20</v>
@@ -2279,17 +2323,17 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I31" s="18" t="str">
         <f t="shared" si="0"/>
@@ -2302,7 +2346,7 @@
         <v>40</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
@@ -2317,10 +2361,10 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
@@ -2335,7 +2379,7 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>38</v>
@@ -2353,10 +2397,10 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
@@ -2371,10 +2415,10 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
@@ -2389,10 +2433,10 @@
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
@@ -2410,7 +2454,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D38" s="13">
         <v>20</v>
@@ -2430,7 +2474,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D39" s="13">
         <v>20</v>
@@ -2450,20 +2494,18 @@
         <v>43</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" s="13"/>
+        <v>52</v>
+      </c>
+      <c r="D40" s="13">
+        <v>1</v>
+      </c>
       <c r="E40" s="13"/>
-      <c r="F40" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>119</v>
-      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
       <c r="H40" s="8"/>
       <c r="I40" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>public int Gender { get; set; }</v>
+        <v>public string Gender { get; set; }</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -2472,7 +2514,7 @@
         <v>44</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
@@ -2490,7 +2532,7 @@
         <v>45</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
@@ -2508,7 +2550,7 @@
         <v>46</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
@@ -2523,7 +2565,7 @@
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>38</v>
@@ -2541,10 +2583,10 @@
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
@@ -2559,7 +2601,7 @@
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>38</v>
@@ -2577,10 +2619,10 @@
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="B47" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
@@ -2595,7 +2637,7 @@
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>38</v>
@@ -2613,10 +2655,10 @@
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
@@ -2641,7 +2683,7 @@
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="11"/>
       <c r="B51" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -2667,7 +2709,7 @@
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="B53" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>38</v>
@@ -2678,14 +2720,14 @@
         <v>34</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
       <c r="B54" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>38</v>
@@ -2696,14 +2738,14 @@
         <v>34</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
       <c r="B55" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>38</v>
@@ -2717,10 +2759,10 @@
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
       <c r="B56" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
@@ -2731,7 +2773,7 @@
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="13"/>
       <c r="B57" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>38</v>
@@ -2745,10 +2787,10 @@
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="B58" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="13"/>
@@ -2759,7 +2801,7 @@
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
       <c r="B59" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>38</v>
@@ -2773,10 +2815,10 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="13"/>
       <c r="B60" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="13"/>
@@ -2797,7 +2839,7 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="11"/>
       <c r="B62" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
@@ -2821,7 +2863,7 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="13"/>
       <c r="B64" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
@@ -2833,7 +2875,7 @@
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
       <c r="B65" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>38</v>
@@ -2844,14 +2886,14 @@
         <v>34</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H65" s="8"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="13"/>
       <c r="B66" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>38</v>
@@ -2862,19 +2904,19 @@
         <v>34</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="13"/>
       <c r="B67" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D67" s="13">
         <v>20</v>
@@ -2887,13 +2929,13 @@
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="13"/>
       <c r="B68" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>97</v>
       </c>
       <c r="E68" s="13"/>
       <c r="F68" s="13"/>
@@ -2903,10 +2945,10 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
       <c r="B69" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C69" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
@@ -2917,7 +2959,7 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
       <c r="B70" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>38</v>
@@ -2931,10 +2973,10 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="13"/>
       <c r="B71" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
@@ -2945,7 +2987,7 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
       <c r="B72" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C72" s="13" t="s">
         <v>38</v>
@@ -2959,10 +3001,10 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
       <c r="B73" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
@@ -2973,7 +3015,7 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="11"/>
       <c r="B74" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
@@ -2999,7 +3041,7 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
       <c r="B76" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
@@ -3008,17 +3050,17 @@
         <v>34</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H76" s="8"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
       <c r="B77" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D77" s="13">
         <v>100</v>
@@ -3031,10 +3073,10 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
       <c r="B78" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D78" s="13">
         <v>500</v>
@@ -3047,10 +3089,10 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
       <c r="B79" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D79" s="13">
         <v>256</v>
@@ -3063,7 +3105,7 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="13"/>
       <c r="B80" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>38</v>
@@ -3077,10 +3119,10 @@
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="13"/>
       <c r="B81" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
@@ -3091,7 +3133,7 @@
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
       <c r="B82" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>38</v>
@@ -3105,10 +3147,10 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
       <c r="B83" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
@@ -3118,28 +3160,28 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D85" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G85" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3152,10 +3194,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3168,7 +3210,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3176,10 +3218,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>148</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3187,10 +3229,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>150</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3198,10 +3240,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>152</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3209,10 +3251,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3220,7 +3262,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3228,34 +3270,45 @@
         <v>6</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="29" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="43"/>
+      <c r="C10" s="25" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="25" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="29" t="s">
         <v>167</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:B11"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
@@ -3266,6 +3319,7 @@
     <hyperlink ref="C8" r:id="rId7"/>
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented Health Check Functionality
</commit_message>
<xml_diff>
--- a/Authorization-Policy-Group-Roles-Permissions.xlsx
+++ b/Authorization-Policy-Group-Roles-Permissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="179">
   <si>
     <t>Admin</t>
   </si>
@@ -406,9 +406,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>ASP.NET Core</t>
-  </si>
-  <si>
     <t>Interface</t>
   </si>
   <si>
@@ -454,9 +451,6 @@
     <t>Versioning</t>
   </si>
   <si>
-    <t>Monolathic Architecture</t>
-  </si>
-  <si>
     <t>SQL Server Local Database With Entity Framework Core</t>
   </si>
   <si>
@@ -542,6 +536,30 @@
   </si>
   <si>
     <t>CHAR</t>
+  </si>
+  <si>
+    <t>HealthCheck</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Self Deployment</t>
+  </si>
+  <si>
+    <t>IIS</t>
+  </si>
+  <si>
+    <t>ASP.NET Core - Monolithic</t>
+  </si>
+  <si>
+    <t>ASP.NET Core - Microservices</t>
+  </si>
+  <si>
+    <t>Monolithic Architecture</t>
+  </si>
+  <si>
+    <t>https://www.stevejgordon.co.uk/cqrs-using-mediatr-asp-net-core</t>
   </si>
 </sst>
 </file>
@@ -585,7 +603,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,6 +631,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -821,10 +845,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1141,9 +1174,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1155,17 +1190,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>124</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1174,184 +1209,243 @@
       <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="14" t="s">
         <v>123</v>
       </c>
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="34" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="C4" s="22"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="35"/>
+      <c r="B5" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="B6" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="21" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="21" t="s">
+      <c r="C10" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="21" t="s">
+      <c r="C11" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="33"/>
+      <c r="B12" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="33"/>
+      <c r="B13" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="33"/>
+      <c r="B14" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="C11" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="C12" s="22"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="22"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="22"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="B15" s="21" t="s">
+      <c r="C16" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="33"/>
+      <c r="B17" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="22"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="21" t="s">
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="33"/>
+      <c r="B18" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="21" t="s">
+      <c r="C18" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
+      <c r="B19" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="22"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="22"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="21" t="s">
-        <v>162</v>
-      </c>
       <c r="C19" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="30"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C20" s="22"/>
+        <v>160</v>
+      </c>
+      <c r="C20" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="30"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
+      <c r="B21" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
+      <c r="B22" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" s="22">
-        <v>1</v>
-      </c>
+      <c r="A23" s="30"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32" t="s">
+        <v>158</v>
+      </c>
       <c r="B24" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="22"/>
+        <v>137</v>
+      </c>
+      <c r="C24" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="32"/>
+      <c r="B25" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" s="22"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="32"/>
+      <c r="B28" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A23:A24"/>
+  <mergeCells count="6">
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A4:A5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C29:C1048576 C1:C3 C5:C26">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:C28">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -1388,41 +1482,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="39" t="s">
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="42" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1435,13 +1529,13 @@
       <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="40"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1467,7 +1561,7 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1491,7 +1585,7 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="37" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1517,7 +1611,7 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="35"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1539,7 +1633,7 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="37" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1563,7 +1657,7 @@
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1679,7 @@
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1860,9 +1954,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1878,16 +1972,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -2096,7 +2190,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>38</v>
@@ -2106,7 +2200,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I13" s="18" t="str">
         <f t="shared" si="1"/>
@@ -2412,7 +2506,7 @@
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I31" s="18" t="str">
         <f t="shared" si="3"/>
@@ -2573,7 +2667,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D40" s="13">
         <v>1</v>
@@ -3405,10 +3499,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3421,7 +3515,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3429,10 +3523,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3440,10 +3534,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3451,10 +3545,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3462,10 +3556,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3473,7 +3567,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3481,39 +3575,48 @@
         <v>6</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="46"/>
+      <c r="C10" s="25" t="s">
         <v>164</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
-      <c r="C10" s="25" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="43"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3531,6 +3634,7 @@
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>